<commit_message>
Pushing test case 319 that caused bug
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2_Frozen/QuerySet2.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2_Frozen/QuerySet2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="824">
   <si>
     <t>Index</t>
   </si>
@@ -2482,6 +2482,15 @@
   </si>
   <si>
     <t>4 whiles</t>
+  </si>
+  <si>
+    <t>assign a; while w; prog_line n;</t>
+  </si>
+  <si>
+    <t>Select a such that Next(a,n) and Next*(n,n) with n=w.stmt#</t>
+  </si>
+  <si>
+    <t>10,16,21,27,31,32</t>
   </si>
 </sst>
 </file>
@@ -2658,53 +2667,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF57BB8A"/>
-          <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE67C73"/>
-          <bgColor rgb="FFE67C73"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF57BB8A"/>
-          <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE67C73"/>
-          <bgColor rgb="FFE67C73"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <b/>
@@ -3290,9 +3253,9 @@
   <dimension ref="A1:G365"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A321" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C336" sqref="C336"/>
+      <selection pane="bottomLeft" activeCell="C318" sqref="C318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9309,11 +9272,21 @@
       <c r="G319" s="16"/>
     </row>
     <row r="320" spans="1:7">
-      <c r="A320" s="6"/>
-      <c r="B320" s="9"/>
-      <c r="C320" s="9"/>
-      <c r="D320" s="14"/>
-      <c r="E320" s="9"/>
+      <c r="A320" s="6">
+        <v>319</v>
+      </c>
+      <c r="B320" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="C320" s="9" t="s">
+        <v>822</v>
+      </c>
+      <c r="D320" s="14" t="s">
+        <v>823</v>
+      </c>
+      <c r="E320" s="9" t="s">
+        <v>776</v>
+      </c>
       <c r="F320" s="16"/>
       <c r="G320" s="16"/>
     </row>
@@ -10196,121 +10169,121 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1 G366:G1048576">
-    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G101">
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:G200">
-    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G102))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102:G200">
-    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G102))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201">
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G201">
-    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202:G251">
-    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202:G251">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G252:G301">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G252))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G252:G301">
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G252))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G302:G311">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G302))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G302:G311">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G302))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G312:G316">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G312))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G312:G316">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G312))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G317:G319">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G317))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G317:G319">
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G317))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G321:G341">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="BUG">
+      <formula>NOT(ISERROR(SEARCH(("BUG"),(G321))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G321:G341">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH(("PASS"),(G321))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G342:G365">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="BUG">
+      <formula>NOT(ISERROR(SEARCH(("BUG"),(G342))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G342:G365">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH(("PASS"),(G342))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G320">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH(("BUG"),(G320))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G320">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH(("PASS"),(G320))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G321:G341">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="BUG">
-      <formula>NOT(ISERROR(SEARCH(("BUG"),(G321))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G321:G341">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH(("PASS"),(G321))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G342:G365">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
-      <formula>NOT(ISERROR(SEARCH(("BUG"),(G342))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G342:G365">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH(("PASS"),(G342))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Update test answer for test 2
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2_Frozen/QuerySet2.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test2_Frozen/QuerySet2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="825">
   <si>
     <t>Index</t>
   </si>
@@ -1017,9 +1017,6 @@
     <t>Underscore Expr NotSameSubTree PartialMatch NoAnswer</t>
   </si>
   <si>
-    <t>Select a pattern a(_, _"14+100*a"_)</t>
-  </si>
-  <si>
     <t>Underscore Expr SameSubTree PartialMatch HasAnswer</t>
   </si>
   <si>
@@ -1317,9 +1314,6 @@
     <t>Select s such that Modifies(s, v) and Uses(s, v)</t>
   </si>
   <si>
-    <t>1,2,3,5,7,8,11,14,15,18,19,23,24,26,28,29,30,33</t>
-  </si>
-  <si>
     <t>InSameStmt ChooseStmt Modifies and Uses SameUnknownVar HasAnswer</t>
   </si>
   <si>
@@ -1338,9 +1332,6 @@
     <t>What variable is modified and used?</t>
   </si>
   <si>
-    <t>assign s; variable v;</t>
-  </si>
-  <si>
     <t>Select a such that Modifies(a, v) and Uses(a, v)</t>
   </si>
   <si>
@@ -1368,9 +1359,6 @@
     <t>Which procedure modifies and uses the same variable?</t>
   </si>
   <si>
-    <t>stmt s1, s2; variable;</t>
-  </si>
-  <si>
     <t>Select s1 such that Modifies(s1, v) and Parent(s1, s2)</t>
   </si>
   <si>
@@ -1956,9 +1944,6 @@
     <t>3 clauses: select p1 calls p1 p2 calls p3 p1 with p3</t>
   </si>
   <si>
-    <t>Four, Five</t>
-  </si>
-  <si>
     <t>4 clauses: select p1 calls p2 p1 with p2 and calls p2 p3 with p3</t>
   </si>
   <si>
@@ -1998,9 +1983,6 @@
     <t>1 Clause: select while 1 synonym (1stArg), given arg; Has answer</t>
   </si>
   <si>
-    <t>calls c;</t>
-  </si>
-  <si>
     <t>Select c such that Next(c, 11)</t>
   </si>
   <si>
@@ -2049,9 +2031,6 @@
     <t>1 Clause: select while 1 synonym (2nd Arg), given arg; Has answer</t>
   </si>
   <si>
-    <t>Select boolean such that Next*(19,19)</t>
-  </si>
-  <si>
     <t>1 clause: same value on both arg, boolean, false</t>
   </si>
   <si>
@@ -2169,9 +2148,6 @@
     <t>Select c such that Next*(a,c) and Next*(w,c)</t>
   </si>
   <si>
-    <t>14,15</t>
-  </si>
-  <si>
     <t>nextstar a c and nextstar w c</t>
   </si>
   <si>
@@ -2181,9 +2157,6 @@
     <t>Select s1 such that Next(s1,s2) and Next(s2,s3)</t>
   </si>
   <si>
-    <t>4,5,11,12,13,14,15,16,17,18,20,21,23,26,27,28,29,30,31,32,35,36</t>
-  </si>
-  <si>
     <t>next s1 s2 and next s2 s3</t>
   </si>
   <si>
@@ -2238,12 +2211,6 @@
     <t>stmt s; while w; constant c;</t>
   </si>
   <si>
-    <t>Select s such that Next*(s,s) with s.stmt# = c.value and Next*(s,w)</t>
-  </si>
-  <si>
-    <t>2,10</t>
-  </si>
-  <si>
     <t>Select a such that Next(a,w) pattern a(_,_"2*h"_)</t>
   </si>
   <si>
@@ -2259,15 +2226,9 @@
     <t>Select v such that Next*(a,w) pattern a(v,_)</t>
   </si>
   <si>
-    <t>g,j,k,m,s,t,u</t>
-  </si>
-  <si>
     <t>next and pattern clause get variables</t>
   </si>
   <si>
-    <t>Select s such that Next*(w,i) pattern w("u",_) and Next*(s,a) with s.stmt# = 31</t>
-  </si>
-  <si>
     <t>next and pattern and with</t>
   </si>
   <si>
@@ -2277,9 +2238,6 @@
     <t>Select s1 such that Next(s1,w) and Next*(s2,w) and Next*(s1,s2)</t>
   </si>
   <si>
-    <t>16,28,31,32</t>
-  </si>
-  <si>
     <t>3 next</t>
   </si>
   <si>
@@ -2289,9 +2247,6 @@
     <t>Select a such that Next(_,a) and Next(a,i) and Next*(a,w) and Next(a,c)</t>
   </si>
   <si>
-    <t>4 next</t>
-  </si>
-  <si>
     <t>1 while, no synonym</t>
   </si>
   <si>
@@ -2358,9 +2313,6 @@
     <t>3 whiles</t>
   </si>
   <si>
-    <t>while w; w1, w2, w3;</t>
-  </si>
-  <si>
     <t>4 whiles</t>
   </si>
   <si>
@@ -2442,9 +2394,6 @@
     <t>10,12,16,21, 27</t>
   </si>
   <si>
-    <t>while w; if I;</t>
-  </si>
-  <si>
     <t>Select v such that Calls(p, "Seven")</t>
   </si>
   <si>
@@ -2479,15 +2428,78 @@
   </si>
   <si>
     <t>1 while, 1 synonym, select all assign</t>
+  </si>
+  <si>
+    <t>Three,Five</t>
+  </si>
+  <si>
+    <t>Four, Five, Six</t>
+  </si>
+  <si>
+    <t>call c;</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Next*(19,19)</t>
+  </si>
+  <si>
+    <t>14,15,28</t>
+  </si>
+  <si>
+    <t>Select s such that Next*(s,s) with s.stmt# = c.value such that Next*(s,w)</t>
+  </si>
+  <si>
+    <t>g,j,k,m,s,t,u,l</t>
+  </si>
+  <si>
+    <t>Select s such that Next*(w,i) pattern w("u",_) such that Next*(s,a) with s.stmt# = 31</t>
+  </si>
+  <si>
+    <t>4 next NoResult</t>
+  </si>
+  <si>
+    <t>10,12</t>
+  </si>
+  <si>
+    <t>Select a pattern a(_, _"100*a"_)</t>
+  </si>
+  <si>
+    <t>while w, w1; variable v;</t>
+  </si>
+  <si>
+    <t>while w, w1, w2, w3;</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>1,2,3,5,7,8,11,13,14,15,18,19,23,24,26,28,29,30,33</t>
+  </si>
+  <si>
+    <t>stmt s1, s2; variable v;</t>
+  </si>
+  <si>
+    <t>1,2,4,5,9,10,11,12,13,14,15,16,17,18,20,21,23,26,27,28,29,30,31,32,35,36</t>
+  </si>
+  <si>
+    <t>2,9,10,14</t>
+  </si>
+  <si>
+    <t>2,10,16,18,21,27,28,31,32</t>
+  </si>
+  <si>
+    <t>stmt s; assign a; while w; if i;</t>
+  </si>
+  <si>
+    <t>10,12,16</t>
+  </si>
+  <si>
+    <t>Select v such that Modifies(a, v) and Uses(a, v)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m\,\ d"/>
-  </numFmts>
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -2599,7 +2611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2658,9 +2670,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3247,9 +3256,9 @@
   <dimension ref="A1:G337"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D318" sqref="D318"/>
+      <selection pane="bottomLeft" activeCell="D296" sqref="D296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3281,10 +3290,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3297,7 +3306,7 @@
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -3305,7 +3314,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3392,13 +3401,13 @@
         <v>111</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>784</v>
+        <v>768</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -3465,16 +3474,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>355</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>356</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -3484,16 +3493,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>358</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>359</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -3506,13 +3515,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D13" s="6">
         <v>3</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -3522,16 +3531,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>363</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>364</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -3544,13 +3553,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -3560,16 +3569,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>367</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>368</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -3582,13 +3591,13 @@
         <v>295</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -3598,16 +3607,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>372</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>373</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -3620,13 +3629,13 @@
         <v>9</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -3636,16 +3645,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>377</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>378</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>32</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -3658,13 +3667,13 @@
         <v>304</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>769</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>380</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>785</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>381</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -3677,13 +3686,13 @@
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>382</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>383</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -3696,13 +3705,13 @@
         <v>21</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -3712,16 +3721,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>386</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>387</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -3731,16 +3740,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>389</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>390</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -3753,13 +3762,13 @@
         <v>10</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -3769,16 +3778,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>394</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>395</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -3788,16 +3797,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>397</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>398</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -3807,16 +3816,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>400</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>401</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -3825,17 +3834,17 @@
       <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>787</v>
+      <c r="B30" s="25" t="s">
+        <v>771</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -3848,13 +3857,13 @@
         <v>24</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -3867,13 +3876,13 @@
         <v>24</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>407</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>408</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
@@ -3883,16 +3892,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>410</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
@@ -3902,16 +3911,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>412</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>413</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
@@ -3921,16 +3930,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>415</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>416</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -3940,16 +3949,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>418</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>419</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -3959,16 +3968,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>476</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>786</v>
+      <c r="D37" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>770</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -3978,16 +3987,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>424</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -4000,13 +4009,13 @@
         <v>5</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -4019,13 +4028,13 @@
         <v>5</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
@@ -4063,7 +4072,7 @@
         <v>7</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -4082,7 +4091,7 @@
         <v>23</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -4101,7 +4110,7 @@
         <v>26</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -4120,7 +4129,7 @@
         <v>29</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -4139,7 +4148,7 @@
         <v>32</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -4158,7 +4167,7 @@
         <v>34</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -4177,7 +4186,7 @@
         <v>99</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -4192,11 +4201,11 @@
       <c r="C49" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="24" t="s">
         <v>182</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -4215,7 +4224,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -4234,7 +4243,7 @@
         <v>8</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -4247,13 +4256,13 @@
         <v>40</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
@@ -4263,16 +4272,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>23</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
@@ -4285,13 +4294,13 @@
         <v>295</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D54" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
@@ -4304,13 +4313,13 @@
         <v>297</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
@@ -4323,13 +4332,13 @@
         <v>301</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -4342,13 +4351,13 @@
         <v>299</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
@@ -4361,13 +4370,13 @@
         <v>168</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>99</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -4380,13 +4389,13 @@
         <v>120</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>34</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -4399,13 +4408,13 @@
         <v>304</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>507</v>
-      </c>
-      <c r="D60" s="27" t="s">
+        <v>503</v>
+      </c>
+      <c r="D60" s="26" t="s">
         <v>182</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
@@ -4424,7 +4433,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
@@ -4438,7 +4447,7 @@
         <v>104</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>105</v>
@@ -4455,7 +4464,7 @@
         <v>106</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>107</v>
@@ -4472,7 +4481,7 @@
         <v>113</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>114</v>
@@ -4488,13 +4497,13 @@
         <v>17</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
@@ -4507,13 +4516,13 @@
         <v>17</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
@@ -4528,8 +4537,8 @@
       <c r="C67" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="25" t="s">
-        <v>788</v>
+      <c r="D67" s="24" t="s">
+        <v>772</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>115</v>
@@ -4545,13 +4554,13 @@
         <v>5</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
@@ -4583,13 +4592,13 @@
         <v>21</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D70" s="13">
         <v>27</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
@@ -4602,13 +4611,13 @@
         <v>24</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
@@ -4621,13 +4630,13 @@
         <v>27</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="D72" s="28" t="s">
-        <v>789</v>
+        <v>519</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>773</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -4640,13 +4649,13 @@
         <v>30</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="D73" s="28" t="s">
-        <v>790</v>
+        <v>521</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>774</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
@@ -4659,13 +4668,13 @@
         <v>36</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D74" s="13">
         <v>27</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
@@ -4700,7 +4709,7 @@
         <v>118</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>119</v>
@@ -4722,7 +4731,7 @@
         <v>7</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
@@ -4738,10 +4747,10 @@
         <v>122</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
@@ -4755,7 +4764,7 @@
         <v>124</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>125</v>
@@ -4772,7 +4781,7 @@
         <v>126</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>127</v>
@@ -4808,7 +4817,7 @@
         <v>129</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>130</v>
@@ -4826,8 +4835,8 @@
       <c r="C83" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D83" s="29" t="s">
-        <v>532</v>
+      <c r="D83" s="28" t="s">
+        <v>528</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>132</v>
@@ -4884,10 +4893,10 @@
         <v>141</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
@@ -4902,11 +4911,11 @@
       <c r="C87" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D87" s="29" t="s">
-        <v>530</v>
+      <c r="D87" s="28" t="s">
+        <v>526</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
@@ -4917,13 +4926,13 @@
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="s">
-        <v>536</v>
-      </c>
-      <c r="D88" s="30" t="s">
-        <v>468</v>
+        <v>532</v>
+      </c>
+      <c r="D88" s="29" t="s">
+        <v>464</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -4933,14 +4942,14 @@
         <v>88</v>
       </c>
       <c r="B89" s="6"/>
-      <c r="C89" s="26" t="s">
-        <v>791</v>
-      </c>
-      <c r="D89" s="25" t="s">
-        <v>467</v>
+      <c r="C89" s="25" t="s">
+        <v>775</v>
+      </c>
+      <c r="D89" s="24" t="s">
+        <v>463</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -4953,13 +4962,13 @@
         <v>17</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -4972,13 +4981,13 @@
         <v>17</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
@@ -4990,14 +4999,14 @@
       <c r="B92" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="26" t="s">
-        <v>792</v>
-      </c>
-      <c r="D92" s="25" t="s">
-        <v>793</v>
+      <c r="C92" s="25" t="s">
+        <v>776</v>
+      </c>
+      <c r="D92" s="24" t="s">
+        <v>777</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -5010,13 +5019,13 @@
         <v>14</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
@@ -5029,7 +5038,7 @@
         <v>17</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>8</v>
@@ -5048,13 +5057,13 @@
         <v>42</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
@@ -5064,16 +5073,16 @@
         <v>95</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
@@ -5083,16 +5092,16 @@
         <v>96</v>
       </c>
       <c r="B97" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>551</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>555</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
@@ -5102,16 +5111,16 @@
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>558</v>
-      </c>
-      <c r="D98" s="25" t="s">
+        <v>554</v>
+      </c>
+      <c r="D98" s="24" t="s">
         <v>13</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
@@ -5121,16 +5130,16 @@
         <v>98</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
@@ -5140,19 +5149,19 @@
         <v>99</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>564</v>
-      </c>
-      <c r="D100" s="25" t="s">
+        <v>560</v>
+      </c>
+      <c r="D100" s="24" t="s">
         <v>13</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>565</v>
-      </c>
-      <c r="F100" s="26" t="s">
-        <v>794</v>
+        <v>561</v>
+      </c>
+      <c r="F100" s="25" t="s">
+        <v>778</v>
       </c>
       <c r="G100" s="6"/>
     </row>
@@ -5161,16 +5170,16 @@
         <v>100</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
@@ -5180,16 +5189,16 @@
         <v>101</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>570</v>
-      </c>
-      <c r="D102" s="25" t="s">
-        <v>795</v>
+        <v>566</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>779</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
@@ -5199,16 +5208,16 @@
         <v>102</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
@@ -5218,16 +5227,16 @@
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>796</v>
+        <v>780</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
@@ -5237,16 +5246,16 @@
         <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
@@ -5256,16 +5265,16 @@
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
@@ -5275,16 +5284,16 @@
         <v>106</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
@@ -5294,16 +5303,16 @@
         <v>107</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
@@ -5316,13 +5325,13 @@
         <v>5</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>799</v>
+        <v>783</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>797</v>
+        <v>781</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>798</v>
+        <v>782</v>
       </c>
       <c r="F109" s="6"/>
       <c r="G109" s="6"/>
@@ -5335,7 +5344,7 @@
         <v>5</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>800</v>
+        <v>784</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>8</v>
@@ -5354,10 +5363,10 @@
         <v>120</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>801</v>
+        <v>785</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>804</v>
+        <v>788</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>230</v>
@@ -5373,10 +5382,10 @@
         <v>120</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>802</v>
+        <v>786</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>233</v>
@@ -5392,13 +5401,13 @@
         <v>123</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>803</v>
+        <v>787</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
@@ -5411,13 +5420,13 @@
         <v>44</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
@@ -5430,13 +5439,13 @@
         <v>44</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D115" s="7" t="s">
         <v>323</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="F115" s="6"/>
       <c r="G115" s="6"/>
@@ -5449,13 +5458,13 @@
         <v>44</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
@@ -5465,16 +5474,16 @@
         <v>116</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D117" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="F117" s="6"/>
       <c r="G117" s="6"/>
@@ -5484,16 +5493,16 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="D118" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
@@ -5503,16 +5512,16 @@
         <v>118</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>804</v>
+        <v>788</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
@@ -5522,16 +5531,16 @@
         <v>119</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D120" s="7" t="s">
         <v>323</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
@@ -5541,16 +5550,16 @@
         <v>120</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
@@ -5561,10 +5570,10 @@
       </c>
       <c r="B122" s="6"/>
       <c r="C122" s="6" t="s">
-        <v>805</v>
+        <v>789</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>105</v>
@@ -5581,7 +5590,7 @@
         <v>143</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>107</v>
@@ -5595,10 +5604,10 @@
       </c>
       <c r="B124" s="6"/>
       <c r="C124" s="6" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>114</v>
@@ -5617,10 +5626,10 @@
         <v>144</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
@@ -5639,7 +5648,7 @@
         <v>13</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
@@ -5655,7 +5664,7 @@
         <v>48</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="E127" s="6"/>
       <c r="F127" s="6"/>
@@ -5757,7 +5766,7 @@
         <v>145</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>806</v>
+        <v>790</v>
       </c>
       <c r="E133" s="6"/>
       <c r="F133" s="6"/>
@@ -5791,7 +5800,7 @@
         <v>146</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E135" s="6"/>
       <c r="F135" s="6"/>
@@ -5887,7 +5896,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>807</v>
+        <v>55</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>147</v>
@@ -6262,7 +6271,7 @@
         <v>137</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>808</v>
+        <v>791</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>34</v>
@@ -6589,7 +6598,7 @@
         <v>0</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="6"/>
@@ -6606,7 +6615,7 @@
         <v>1</v>
       </c>
       <c r="E179" s="6" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F179" s="6"/>
       <c r="G179" s="6"/>
@@ -6638,10 +6647,10 @@
         <v>14</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="E181" s="6" t="s">
         <v>213</v>
@@ -6733,7 +6742,7 @@
         <v>14</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="D186" s="14" t="s">
         <v>8</v>
@@ -6777,7 +6786,7 @@
         <v>8</v>
       </c>
       <c r="E188" s="6" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="F188" s="6"/>
       <c r="G188" s="6"/>
@@ -6796,7 +6805,7 @@
         <v>159</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="F189" s="6"/>
       <c r="G189" s="6"/>
@@ -6815,7 +6824,7 @@
         <v>154</v>
       </c>
       <c r="E190" s="6" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="F190" s="6"/>
       <c r="G190" s="6"/>
@@ -6828,13 +6837,13 @@
         <v>162</v>
       </c>
       <c r="C191" s="6" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="D191" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="F191" s="6"/>
       <c r="G191" s="6"/>
@@ -6844,16 +6853,16 @@
         <v>191</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="F192" s="6"/>
       <c r="G192" s="6"/>
@@ -6863,19 +6872,19 @@
         <v>192</v>
       </c>
       <c r="B193" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="C193" s="6" t="s">
         <v>622</v>
-      </c>
-      <c r="C193" s="6" t="s">
-        <v>626</v>
       </c>
       <c r="D193" s="6" t="s">
         <v>156</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="F193" s="6" t="s">
-        <v>809</v>
+        <v>792</v>
       </c>
       <c r="G193" s="6"/>
     </row>
@@ -6884,19 +6893,19 @@
         <v>193</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D194" s="6" t="s">
         <v>161</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="F194" s="6" t="s">
-        <v>810</v>
+        <v>793</v>
       </c>
       <c r="G194" s="6"/>
     </row>
@@ -6905,19 +6914,19 @@
         <v>194</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="D195" s="6" t="s">
         <v>161</v>
       </c>
       <c r="E195" s="6" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="F195" s="6" t="s">
-        <v>810</v>
+        <v>793</v>
       </c>
       <c r="G195" s="6"/>
     </row>
@@ -6926,16 +6935,16 @@
         <v>195</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="F196" s="6"/>
       <c r="G196" s="6"/>
@@ -6945,16 +6954,16 @@
         <v>196</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C197" s="6" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D197" s="6" t="s">
         <v>156</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="F197" s="6"/>
       <c r="G197" s="6"/>
@@ -6964,16 +6973,16 @@
         <v>197</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C198" s="6" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="D198" s="6" t="s">
         <v>161</v>
       </c>
       <c r="E198" s="6" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="6"/>
@@ -7236,7 +7245,7 @@
         <v>253</v>
       </c>
       <c r="D212" s="7" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="E212" s="6" t="s">
         <v>254</v>
@@ -7277,7 +7286,7 @@
         <v>154</v>
       </c>
       <c r="E214" s="6" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="F214" s="6"/>
       <c r="G214" s="6"/>
@@ -7296,7 +7305,7 @@
         <v>212</v>
       </c>
       <c r="E215" s="6" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="F215" s="6"/>
       <c r="G215" s="6"/>
@@ -7315,7 +7324,7 @@
         <v>260</v>
       </c>
       <c r="E216" s="6" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="F216" s="6"/>
       <c r="G216" s="6"/>
@@ -7328,13 +7337,13 @@
         <v>138</v>
       </c>
       <c r="C217" s="6" t="s">
-        <v>811</v>
+        <v>794</v>
       </c>
       <c r="D217" s="6" t="s">
         <v>161</v>
       </c>
       <c r="E217" s="6" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="F217" s="6"/>
       <c r="G217" s="6"/>
@@ -7344,16 +7353,16 @@
         <v>217</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C218" s="6" t="s">
-        <v>812</v>
+        <v>795</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>212</v>
+        <v>803</v>
       </c>
       <c r="E218" s="6" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="F218" s="6"/>
       <c r="G218" s="6"/>
@@ -7363,16 +7372,16 @@
         <v>218</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D219" s="6" t="s">
         <v>154</v>
       </c>
       <c r="E219" s="6" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="F219" s="6"/>
       <c r="G219" s="6"/>
@@ -7382,16 +7391,16 @@
         <v>219</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>813</v>
+        <v>796</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>645</v>
+        <v>804</v>
       </c>
       <c r="E220" s="6" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F220" s="6"/>
       <c r="G220" s="6"/>
@@ -7401,16 +7410,16 @@
         <v>220</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="D221" s="6" t="s">
         <v>239</v>
       </c>
       <c r="E221" s="6" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="F221" s="6"/>
       <c r="G221" s="6"/>
@@ -7459,13 +7468,13 @@
       </c>
       <c r="B224" s="15"/>
       <c r="C224" s="15" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="D224" s="14" t="b">
         <v>1</v>
       </c>
       <c r="E224" s="15" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="F224" s="16"/>
       <c r="G224" s="17"/>
@@ -7535,13 +7544,13 @@
         <v>21</v>
       </c>
       <c r="C228" s="15" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="D228" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E228" s="15" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="F228" s="16"/>
       <c r="G228" s="17"/>
@@ -7554,13 +7563,13 @@
         <v>21</v>
       </c>
       <c r="C229" s="15" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="D229" s="19">
         <v>16</v>
       </c>
       <c r="E229" s="15" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="F229" s="16"/>
       <c r="G229" s="17"/>
@@ -7573,13 +7582,13 @@
         <v>24</v>
       </c>
       <c r="C230" s="15" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="D230" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E230" s="15" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="F230" s="16"/>
       <c r="G230" s="17"/>
@@ -7592,13 +7601,13 @@
         <v>24</v>
       </c>
       <c r="C231" s="15" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="D231" s="19">
         <v>11</v>
       </c>
       <c r="E231" s="15" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="F231" s="16"/>
       <c r="G231" s="17"/>
@@ -7608,16 +7617,16 @@
         <v>231</v>
       </c>
       <c r="B232" s="15" t="s">
-        <v>659</v>
+        <v>805</v>
       </c>
       <c r="C232" s="15" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="D232" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E232" s="15" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="F232" s="16"/>
       <c r="G232" s="17"/>
@@ -7627,16 +7636,16 @@
         <v>232</v>
       </c>
       <c r="B233" s="15" t="s">
-        <v>659</v>
+        <v>805</v>
       </c>
       <c r="C233" s="15" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="D233" s="19" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="E233" s="15" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="F233" s="16"/>
       <c r="G233" s="17"/>
@@ -7649,13 +7658,13 @@
         <v>27</v>
       </c>
       <c r="C234" s="15" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="D234" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E234" s="15" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="F234" s="16"/>
       <c r="G234" s="17"/>
@@ -7668,13 +7677,13 @@
         <v>27</v>
       </c>
       <c r="C235" s="15" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="D235" s="19">
         <v>13</v>
       </c>
       <c r="E235" s="15" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="F235" s="16"/>
       <c r="G235" s="17"/>
@@ -7744,13 +7753,13 @@
         <v>21</v>
       </c>
       <c r="C239" s="15" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="D239" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E239" s="15" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="F239" s="16"/>
       <c r="G239" s="17"/>
@@ -7763,13 +7772,13 @@
         <v>21</v>
       </c>
       <c r="C240" s="15" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="D240" s="19">
         <v>12</v>
       </c>
       <c r="E240" s="15" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="F240" s="16"/>
       <c r="G240" s="17"/>
@@ -7782,13 +7791,13 @@
         <v>24</v>
       </c>
       <c r="C241" s="15" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="D241" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E241" s="15" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="F241" s="16"/>
       <c r="G241" s="17"/>
@@ -7801,13 +7810,13 @@
         <v>24</v>
       </c>
       <c r="C242" s="15" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="D242" s="19">
         <v>11</v>
       </c>
       <c r="E242" s="15" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="F242" s="16"/>
       <c r="G242" s="17"/>
@@ -7856,13 +7865,13 @@
       </c>
       <c r="B245" s="15"/>
       <c r="C245" s="15" t="s">
-        <v>676</v>
+        <v>806</v>
       </c>
       <c r="D245" s="14" t="b">
         <v>0</v>
       </c>
       <c r="E245" s="15" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="F245" s="16"/>
       <c r="G245" s="17"/>
@@ -7873,13 +7882,13 @@
       </c>
       <c r="B246" s="15"/>
       <c r="C246" s="15" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="D246" s="14" t="b">
         <v>1</v>
       </c>
       <c r="E246" s="15" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="F246" s="16"/>
       <c r="G246" s="17"/>
@@ -7933,7 +7942,7 @@
         <v>282</v>
       </c>
       <c r="D249" s="14" t="s">
-        <v>814</v>
+        <v>797</v>
       </c>
       <c r="E249" s="15" t="s">
         <v>265</v>
@@ -7971,7 +7980,7 @@
         <v>284</v>
       </c>
       <c r="D251" s="19" t="s">
-        <v>815</v>
+        <v>798</v>
       </c>
       <c r="E251" s="15" t="s">
         <v>267</v>
@@ -8028,7 +8037,7 @@
         <v>287</v>
       </c>
       <c r="D254" s="19" t="s">
-        <v>816</v>
+        <v>799</v>
       </c>
       <c r="E254" s="15" t="s">
         <v>84</v>
@@ -8341,16 +8350,16 @@
         <v>270</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="D271" s="19" t="s">
         <v>269</v>
       </c>
       <c r="E271" s="15" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="F271" s="16"/>
       <c r="G271" s="17"/>
@@ -8360,16 +8369,16 @@
         <v>271</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="D272" s="19" t="s">
         <v>277</v>
       </c>
       <c r="E272" s="15" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="F272" s="16"/>
       <c r="G272" s="17"/>
@@ -8382,13 +8391,13 @@
         <v>5</v>
       </c>
       <c r="C273" s="9" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="D273" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E273" s="15" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="F273" s="16"/>
       <c r="G273" s="17"/>
@@ -8401,13 +8410,13 @@
         <v>5</v>
       </c>
       <c r="C274" s="9" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
       <c r="D274" s="14" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="E274" s="15" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="F274" s="16"/>
       <c r="G274" s="17"/>
@@ -8420,13 +8429,13 @@
         <v>5</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
       <c r="D275" s="14">
         <v>13</v>
       </c>
       <c r="E275" s="9" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="F275" s="16"/>
       <c r="G275" s="16"/>
@@ -8439,13 +8448,13 @@
         <v>5</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="D276" s="14">
         <v>13</v>
       </c>
       <c r="E276" s="9" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
       <c r="F276" s="16"/>
       <c r="G276" s="16"/>
@@ -8458,13 +8467,13 @@
         <v>5</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="D277" s="14" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="E277" s="9" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="F277" s="16"/>
       <c r="G277" s="16"/>
@@ -8474,16 +8483,16 @@
         <v>277</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="D278" s="14" t="s">
-        <v>817</v>
+        <v>800</v>
       </c>
       <c r="E278" s="9" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="F278" s="16"/>
       <c r="G278" s="16"/>
@@ -8493,16 +8502,16 @@
         <v>278</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="D279" s="14" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="E279" s="9" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="F279" s="16"/>
       <c r="G279" s="16"/>
@@ -8512,16 +8521,16 @@
         <v>279</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="D280" s="14" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="E280" s="9" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="F280" s="16"/>
       <c r="G280" s="16"/>
@@ -8531,16 +8540,16 @@
         <v>280</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="D281" s="14" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="E281" s="9" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="F281" s="16"/>
       <c r="G281" s="16"/>
@@ -8550,16 +8559,16 @@
         <v>281</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="D282" s="14" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="E282" s="9" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="F282" s="16"/>
       <c r="G282" s="16"/>
@@ -8572,13 +8581,13 @@
         <v>10</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="D283" s="14" t="s">
-        <v>818</v>
+        <v>801</v>
       </c>
       <c r="E283" s="9" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="F283" s="16"/>
       <c r="G283" s="16"/>
@@ -8588,16 +8597,16 @@
         <v>283</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="D284" s="14">
         <v>12</v>
       </c>
       <c r="E284" s="9" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="F284" s="16"/>
       <c r="G284" s="16"/>
@@ -8607,16 +8616,16 @@
         <v>284</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>715</v>
+        <v>708</v>
       </c>
       <c r="D285" s="14" t="s">
-        <v>716</v>
+        <v>807</v>
       </c>
       <c r="E285" s="9" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="F285" s="16"/>
       <c r="G285" s="16"/>
@@ -8626,16 +8635,16 @@
         <v>285</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="D286" s="14" t="s">
-        <v>720</v>
+        <v>819</v>
       </c>
       <c r="E286" s="9" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="F286" s="16"/>
       <c r="G286" s="16"/>
@@ -8645,16 +8654,16 @@
         <v>286</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="D287" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E287" s="9" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="F287" s="16"/>
       <c r="G287" s="16"/>
@@ -8664,16 +8673,16 @@
         <v>287</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="D288" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E288" s="9" t="s">
-        <v>726</v>
+        <v>717</v>
       </c>
       <c r="F288" s="16"/>
       <c r="G288" s="16"/>
@@ -8683,16 +8692,16 @@
         <v>288</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="D289" s="14" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E289" s="9" t="s">
-        <v>729</v>
+        <v>720</v>
       </c>
       <c r="F289" s="16"/>
       <c r="G289" s="16"/>
@@ -8702,16 +8711,16 @@
         <v>289</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="D290" s="14" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="E290" s="9" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
       <c r="F290" s="16"/>
       <c r="G290" s="16"/>
@@ -8721,16 +8730,16 @@
         <v>290</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
       <c r="D291" s="14" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="E291" s="9" t="s">
-        <v>736</v>
+        <v>727</v>
       </c>
       <c r="F291" s="16"/>
       <c r="G291" s="16"/>
@@ -8740,16 +8749,16 @@
         <v>291</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>781</v>
+        <v>765</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>782</v>
+        <v>766</v>
       </c>
       <c r="D292" s="14" t="s">
-        <v>783</v>
+        <v>767</v>
       </c>
       <c r="E292" s="9" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="F292" s="16"/>
       <c r="G292" s="16"/>
@@ -8759,16 +8768,16 @@
         <v>292</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>738</v>
+        <v>729</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>739</v>
+        <v>808</v>
       </c>
       <c r="D293" s="14" t="s">
-        <v>740</v>
+        <v>820</v>
       </c>
       <c r="E293" s="9" t="s">
-        <v>737</v>
+        <v>728</v>
       </c>
       <c r="F293" s="16"/>
       <c r="G293" s="16"/>
@@ -8781,13 +8790,13 @@
         <v>10</v>
       </c>
       <c r="C294" s="9" t="s">
-        <v>741</v>
+        <v>730</v>
       </c>
       <c r="D294" s="14" t="s">
-        <v>742</v>
+        <v>731</v>
       </c>
       <c r="E294" s="9" t="s">
-        <v>743</v>
+        <v>732</v>
       </c>
       <c r="F294" s="16"/>
       <c r="G294" s="16"/>
@@ -8797,16 +8806,16 @@
         <v>294</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>744</v>
+        <v>733</v>
       </c>
       <c r="C295" s="9" t="s">
-        <v>745</v>
+        <v>734</v>
       </c>
       <c r="D295" s="14" t="s">
-        <v>746</v>
+        <v>809</v>
       </c>
       <c r="E295" s="9" t="s">
-        <v>747</v>
+        <v>735</v>
       </c>
       <c r="F295" s="16"/>
       <c r="G295" s="16"/>
@@ -8816,16 +8825,16 @@
         <v>295</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>423</v>
+        <v>822</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>748</v>
+        <v>810</v>
       </c>
       <c r="D296" s="14">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E296" s="9" t="s">
-        <v>749</v>
+        <v>736</v>
       </c>
       <c r="F296" s="16"/>
       <c r="G296" s="16"/>
@@ -8835,16 +8844,16 @@
         <v>296</v>
       </c>
       <c r="B297" s="9" t="s">
-        <v>750</v>
+        <v>737</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>751</v>
+        <v>738</v>
       </c>
       <c r="D297" s="14" t="s">
-        <v>752</v>
+        <v>821</v>
       </c>
       <c r="E297" s="9" t="s">
-        <v>753</v>
+        <v>739</v>
       </c>
       <c r="F297" s="16"/>
       <c r="G297" s="16"/>
@@ -8854,16 +8863,16 @@
         <v>297</v>
       </c>
       <c r="B298" s="9" t="s">
-        <v>754</v>
+        <v>740</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>755</v>
-      </c>
-      <c r="D298" s="14">
-        <v>12</v>
+        <v>741</v>
+      </c>
+      <c r="D298" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="E298" s="9" t="s">
-        <v>756</v>
+        <v>811</v>
       </c>
       <c r="F298" s="16"/>
       <c r="G298" s="16"/>
@@ -8977,8 +8986,8 @@
       <c r="C304" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="D304" s="24">
-        <v>43020</v>
+      <c r="D304" s="7" t="s">
+        <v>812</v>
       </c>
       <c r="E304" s="6" t="s">
         <v>329</v>
@@ -9013,13 +9022,13 @@
         <v>21</v>
       </c>
       <c r="C306" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="D306" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E306" s="6" t="s">
         <v>332</v>
-      </c>
-      <c r="D306" s="6">
-        <v>12</v>
-      </c>
-      <c r="E306" s="6" t="s">
-        <v>333</v>
       </c>
       <c r="F306" s="6"/>
       <c r="G306" s="6"/>
@@ -9032,13 +9041,13 @@
         <v>21</v>
       </c>
       <c r="C307" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D307" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E307" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F307" s="6"/>
       <c r="G307" s="6"/>
@@ -9051,13 +9060,13 @@
         <v>21</v>
       </c>
       <c r="C308" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D308" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E308" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F308" s="6"/>
       <c r="G308" s="6"/>
@@ -9070,13 +9079,13 @@
         <v>44</v>
       </c>
       <c r="C309" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D309" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="D309" s="6" t="s">
+      <c r="E309" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="E309" s="6" t="s">
-        <v>340</v>
       </c>
       <c r="F309" s="6"/>
       <c r="G309" s="6"/>
@@ -9089,13 +9098,13 @@
         <v>44</v>
       </c>
       <c r="C310" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="D310" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="D310" s="6" t="s">
+      <c r="E310" s="6" t="s">
         <v>342</v>
-      </c>
-      <c r="E310" s="6" t="s">
-        <v>343</v>
       </c>
       <c r="F310" s="6"/>
       <c r="G310" s="6"/>
@@ -9108,13 +9117,13 @@
         <v>44</v>
       </c>
       <c r="C311" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D311" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E311" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F311" s="6"/>
       <c r="G311" s="6"/>
@@ -9127,13 +9136,13 @@
         <v>24</v>
       </c>
       <c r="C312" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D312" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E312" s="6" t="s">
-        <v>757</v>
+        <v>742</v>
       </c>
       <c r="F312" s="6"/>
       <c r="G312" s="6"/>
@@ -9146,13 +9155,13 @@
         <v>24</v>
       </c>
       <c r="C313" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D313" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E313" s="6" t="s">
-        <v>758</v>
+        <v>743</v>
       </c>
       <c r="F313" s="6"/>
       <c r="G313" s="6"/>
@@ -9165,13 +9174,13 @@
         <v>24</v>
       </c>
       <c r="C314" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D314" s="6">
         <v>9</v>
       </c>
       <c r="E314" s="6" t="s">
-        <v>759</v>
+        <v>744</v>
       </c>
       <c r="F314" s="6"/>
       <c r="G314" s="6"/>
@@ -9184,13 +9193,13 @@
         <v>45</v>
       </c>
       <c r="C315" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D315" s="6" t="s">
-        <v>760</v>
+        <v>745</v>
       </c>
       <c r="E315" s="6" t="s">
-        <v>761</v>
+        <v>746</v>
       </c>
       <c r="F315" s="6"/>
       <c r="G315" s="6"/>
@@ -9203,13 +9212,13 @@
         <v>45</v>
       </c>
       <c r="C316" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D316" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E316" s="6" t="s">
-        <v>762</v>
+        <v>747</v>
       </c>
       <c r="F316" s="6"/>
       <c r="G316" s="6"/>
@@ -9219,16 +9228,16 @@
         <v>316</v>
       </c>
       <c r="B317" s="6" t="s">
-        <v>763</v>
+        <v>748</v>
       </c>
       <c r="C317" s="6" t="s">
-        <v>764</v>
+        <v>749</v>
       </c>
       <c r="D317" s="7" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E317" s="6" t="s">
-        <v>765</v>
+        <v>750</v>
       </c>
       <c r="F317" s="6"/>
       <c r="G317" s="6"/>
@@ -9238,16 +9247,16 @@
         <v>317</v>
       </c>
       <c r="B318" s="6" t="s">
-        <v>766</v>
+        <v>751</v>
       </c>
       <c r="C318" s="6" t="s">
-        <v>767</v>
-      </c>
-      <c r="D318" s="31" t="s">
+        <v>752</v>
+      </c>
+      <c r="D318" s="30" t="s">
         <v>23</v>
       </c>
       <c r="E318" s="6" t="s">
-        <v>819</v>
+        <v>802</v>
       </c>
       <c r="F318" s="6"/>
       <c r="G318" s="6"/>
@@ -9257,16 +9266,16 @@
         <v>318</v>
       </c>
       <c r="B319" s="6" t="s">
-        <v>768</v>
+        <v>753</v>
       </c>
       <c r="C319" s="6" t="s">
-        <v>769</v>
+        <v>754</v>
       </c>
       <c r="D319" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E319" s="6" t="s">
-        <v>761</v>
+        <v>746</v>
       </c>
       <c r="F319" s="6"/>
       <c r="G319" s="6"/>
@@ -9276,16 +9285,16 @@
         <v>319</v>
       </c>
       <c r="B320" s="6" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
       <c r="C320" s="6" t="s">
-        <v>771</v>
+        <v>756</v>
       </c>
       <c r="D320" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E320" s="6" t="s">
-        <v>772</v>
+        <v>757</v>
       </c>
       <c r="F320" s="6"/>
       <c r="G320" s="6"/>
@@ -9295,16 +9304,16 @@
         <v>320</v>
       </c>
       <c r="B321" s="6" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
       <c r="C321" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D321" s="6">
         <v>1</v>
       </c>
       <c r="E321" s="6" t="s">
-        <v>773</v>
+        <v>758</v>
       </c>
       <c r="F321" s="6"/>
       <c r="G321" s="6"/>
@@ -9314,16 +9323,16 @@
         <v>321</v>
       </c>
       <c r="B322" s="6" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
       <c r="C322" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D322" s="6">
         <v>9</v>
       </c>
       <c r="E322" s="6" t="s">
-        <v>773</v>
+        <v>758</v>
       </c>
       <c r="F322" s="6"/>
       <c r="G322" s="6"/>
@@ -9333,16 +9342,16 @@
         <v>322</v>
       </c>
       <c r="B323" s="6" t="s">
-        <v>770</v>
+        <v>814</v>
       </c>
       <c r="C323" s="6" t="s">
-        <v>774</v>
+        <v>759</v>
       </c>
       <c r="D323" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E323" s="6" t="s">
-        <v>775</v>
+        <v>760</v>
       </c>
       <c r="F323" s="6"/>
       <c r="G323" s="6"/>
@@ -9352,16 +9361,16 @@
         <v>323</v>
       </c>
       <c r="B324" s="6" t="s">
-        <v>770</v>
+        <v>814</v>
       </c>
       <c r="C324" s="6" t="s">
-        <v>776</v>
+        <v>761</v>
       </c>
       <c r="D324" s="7" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="E324" s="6" t="s">
-        <v>775</v>
+        <v>760</v>
       </c>
       <c r="F324" s="6"/>
       <c r="G324" s="6"/>
@@ -9371,16 +9380,16 @@
         <v>324</v>
       </c>
       <c r="B325" s="6" t="s">
-        <v>777</v>
+        <v>762</v>
       </c>
       <c r="C325" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D325" s="6">
         <v>1</v>
       </c>
       <c r="E325" s="6" t="s">
-        <v>778</v>
+        <v>763</v>
       </c>
       <c r="F325" s="6"/>
       <c r="G325" s="6"/>
@@ -9390,16 +9399,16 @@
         <v>325</v>
       </c>
       <c r="B326" s="6" t="s">
-        <v>779</v>
+        <v>815</v>
       </c>
       <c r="C326" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D326" s="6">
         <v>1</v>
       </c>
       <c r="E326" s="6" t="s">
-        <v>780</v>
+        <v>764</v>
       </c>
       <c r="F326" s="6"/>
       <c r="G326" s="6"/>
@@ -9412,13 +9421,13 @@
         <v>5</v>
       </c>
       <c r="C327" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="D327" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="E327" s="6" t="s">
         <v>426</v>
-      </c>
-      <c r="D327" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="E327" s="6" t="s">
-        <v>427</v>
       </c>
       <c r="F327" s="6"/>
       <c r="G327" s="6"/>
@@ -9428,16 +9437,16 @@
         <v>327</v>
       </c>
       <c r="B328" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C328" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="C328" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="D328" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E328" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F328" s="6"/>
       <c r="G328" s="6"/>
@@ -9450,16 +9459,16 @@
         <v>120</v>
       </c>
       <c r="C329" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D329" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="E329" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="D329" s="7" t="s">
+      <c r="F329" s="6" t="s">
         <v>432</v>
-      </c>
-      <c r="E329" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="F329" s="6" t="s">
-        <v>434</v>
       </c>
       <c r="G329" s="6"/>
     </row>
@@ -9471,16 +9480,16 @@
         <v>120</v>
       </c>
       <c r="C330" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="D330" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="E330" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="D330" s="7" t="s">
+      <c r="F330" s="6" t="s">
         <v>436</v>
-      </c>
-      <c r="E330" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="F330" s="6" t="s">
-        <v>438</v>
       </c>
       <c r="G330" s="6"/>
     </row>
@@ -9489,19 +9498,19 @@
         <v>330</v>
       </c>
       <c r="B331" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C331" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D331" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="E331" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="F331" s="6" t="s">
         <v>439</v>
-      </c>
-      <c r="C331" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="D331" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="E331" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="F331" s="6" t="s">
-        <v>442</v>
       </c>
       <c r="G331" s="6"/>
     </row>
@@ -9510,19 +9519,19 @@
         <v>331</v>
       </c>
       <c r="B332" s="6" t="s">
-        <v>439</v>
+        <v>44</v>
       </c>
       <c r="C332" s="6" t="s">
-        <v>440</v>
+        <v>824</v>
       </c>
       <c r="D332" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E332" s="6" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F332" s="6" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G332" s="6"/>
     </row>
@@ -9534,16 +9543,16 @@
         <v>46</v>
       </c>
       <c r="C333" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="D333" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="E333" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="F333" s="6" t="s">
         <v>445</v>
-      </c>
-      <c r="D333" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="E333" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="F333" s="6" t="s">
-        <v>448</v>
       </c>
       <c r="G333" s="6"/>
     </row>
@@ -9552,19 +9561,19 @@
         <v>333</v>
       </c>
       <c r="B334" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="C334" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D334" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="E334" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="F334" s="6" t="s">
         <v>449</v>
-      </c>
-      <c r="C334" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="D334" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="E334" s="6" t="s">
-        <v>452</v>
-      </c>
-      <c r="F334" s="6" t="s">
-        <v>453</v>
       </c>
       <c r="G334" s="6"/>
     </row>
@@ -9573,19 +9582,19 @@
         <v>334</v>
       </c>
       <c r="B335" s="6" t="s">
-        <v>449</v>
+        <v>818</v>
       </c>
       <c r="C335" s="6" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D335" s="7" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E335" s="6" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F335" s="6" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G335" s="6"/>
     </row>
@@ -9594,19 +9603,19 @@
         <v>335</v>
       </c>
       <c r="B336" s="6" t="s">
-        <v>449</v>
+        <v>818</v>
       </c>
       <c r="C336" s="6" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D336" s="7" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="E336" s="6" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="F336" s="6" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G336" s="6"/>
     </row>
@@ -9615,19 +9624,19 @@
         <v>336</v>
       </c>
       <c r="B337" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D337" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E337" s="6" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="F337" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="G337" s="6"/>
     </row>

</xml_diff>